<commit_message>
Provided estimated P test
</commit_message>
<xml_diff>
--- a/figures/results/accuracy_results.xlsx
+++ b/figures/results/accuracy_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fast_files\GitHub\VUB-BCI-thesis\figures\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3CFBFB-472F-4612-9FEE-75108817D160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725099BC-9F77-459E-BB42-6880B39C66F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{DBF0CAC8-621F-4ADA-9356-953CB796B9C0}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DBF0CAC8-621F-4ADA-9356-953CB796B9C0}"/>
   </bookViews>
   <sheets>
     <sheet name="intersubject-more-data" sheetId="13" r:id="rId1"/>
@@ -1011,27 +1011,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1044,13 +1023,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1071,10 +1071,10 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1393,7 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F0558A-9C1B-4287-9C60-9E9EA65C4ADE}">
   <dimension ref="F8:AJ21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z13" sqref="Z13:AC13"/>
     </sheetView>
   </sheetViews>
@@ -1500,18 +1500,18 @@
       <c r="X9" s="19">
         <v>33</v>
       </c>
-      <c r="Z9" s="33" t="s">
+      <c r="Z9" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="34"/>
-      <c r="AC9" s="35"/>
-      <c r="AE9" s="33" t="s">
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="28"/>
+      <c r="AE9" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="AF9" s="34"/>
-      <c r="AG9" s="34"/>
-      <c r="AH9" s="35"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="28"/>
       <c r="AI9" s="24"/>
       <c r="AJ9" s="24"/>
     </row>
@@ -1571,20 +1571,20 @@
       <c r="X10" s="18">
         <v>182</v>
       </c>
-      <c r="Z10" s="32">
+      <c r="Z10" s="25">
         <f>AVERAGE((I10,I16,I19))</f>
         <v>72.111168131919456</v>
       </c>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="32"/>
-      <c r="AC10" s="32"/>
-      <c r="AE10" s="32">
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AE10" s="25">
         <f>_xlfn.STDEV.P((I10,I16,I19))</f>
         <v>9.4283676536094951</v>
       </c>
-      <c r="AF10" s="32"/>
-      <c r="AG10" s="32"/>
-      <c r="AH10" s="32"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="25"/>
       <c r="AI10" s="24"/>
       <c r="AJ10" s="24"/>
     </row>
@@ -1644,20 +1644,20 @@
       <c r="X11" s="18">
         <v>202</v>
       </c>
-      <c r="Z11" s="26">
+      <c r="Z11" s="29">
         <f>AVERAGE((I11,I15,I20))</f>
         <v>73.087791079094529</v>
       </c>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="28"/>
-      <c r="AE11" s="26">
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="31"/>
+      <c r="AE11" s="29">
         <f>_xlfn.STDEV.P((I11,I15,I20))</f>
         <v>10.919455594589914</v>
       </c>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="28"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="31"/>
       <c r="AI11" s="24"/>
       <c r="AJ11" s="24"/>
     </row>
@@ -1717,20 +1717,20 @@
       <c r="X12" s="18">
         <v>204</v>
       </c>
-      <c r="Z12" s="29">
+      <c r="Z12" s="33">
         <f>AVERAGE((I12))</f>
         <v>74.479166666666657</v>
       </c>
-      <c r="AA12" s="30"/>
-      <c r="AB12" s="30"/>
-      <c r="AC12" s="31"/>
-      <c r="AE12" s="29">
+      <c r="AA12" s="34"/>
+      <c r="AB12" s="34"/>
+      <c r="AC12" s="35"/>
+      <c r="AE12" s="33">
         <f>_xlfn.STDEV.P((I12))</f>
         <v>0</v>
       </c>
-      <c r="AF12" s="30"/>
-      <c r="AG12" s="30"/>
-      <c r="AH12" s="31"/>
+      <c r="AF12" s="34"/>
+      <c r="AG12" s="34"/>
+      <c r="AH12" s="35"/>
       <c r="AI12" s="24"/>
       <c r="AJ12" s="24"/>
     </row>
@@ -1790,20 +1790,20 @@
       <c r="X13" s="18">
         <v>240</v>
       </c>
-      <c r="Z13" s="26">
+      <c r="Z13" s="29">
         <f>AVERAGE((I13,I17,I21))</f>
         <v>79.071162878725843</v>
       </c>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="28"/>
-      <c r="AE13" s="26">
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="31"/>
+      <c r="AE13" s="29">
         <f>_xlfn.STDEV.P((I13,I17,I21))</f>
         <v>9.4164146166196723</v>
       </c>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="28"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="31"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
     </row>
@@ -1825,15 +1825,15 @@
       <c r="V14" s="18"/>
       <c r="W14" s="18"/>
       <c r="X14" s="18"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="25"/>
-      <c r="AC14" s="25"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="32"/>
       <c r="AD14" s="24"/>
-      <c r="AE14" s="25"/>
-      <c r="AF14" s="25"/>
-      <c r="AG14" s="25"/>
-      <c r="AH14" s="25"/>
+      <c r="AE14" s="32"/>
+      <c r="AF14" s="32"/>
+      <c r="AG14" s="32"/>
+      <c r="AH14" s="32"/>
       <c r="AI14" s="24"/>
       <c r="AJ14" s="24"/>
     </row>
@@ -1893,15 +1893,15 @@
       <c r="X15" s="18">
         <v>104</v>
       </c>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
+      <c r="Z15" s="32"/>
+      <c r="AA15" s="32"/>
+      <c r="AB15" s="32"/>
+      <c r="AC15" s="32"/>
       <c r="AD15" s="24"/>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="25"/>
-      <c r="AH15" s="25"/>
+      <c r="AE15" s="32"/>
+      <c r="AF15" s="32"/>
+      <c r="AG15" s="32"/>
+      <c r="AH15" s="32"/>
       <c r="AI15" s="24"/>
       <c r="AJ15" s="24"/>
     </row>
@@ -2222,12 +2222,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="Z10:AC10"/>
-    <mergeCell ref="AE10:AH10"/>
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="AE9:AH9"/>
-    <mergeCell ref="Z13:AC13"/>
-    <mergeCell ref="AE13:AH13"/>
     <mergeCell ref="Z14:AC14"/>
     <mergeCell ref="AE14:AH14"/>
     <mergeCell ref="Z15:AC15"/>
@@ -2236,6 +2230,12 @@
     <mergeCell ref="AE11:AH11"/>
     <mergeCell ref="Z12:AC12"/>
     <mergeCell ref="AE12:AH12"/>
+    <mergeCell ref="Z10:AC10"/>
+    <mergeCell ref="AE10:AH10"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="AE9:AH9"/>
+    <mergeCell ref="Z13:AC13"/>
+    <mergeCell ref="AE13:AH13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2246,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88097A8A-907F-41F3-B591-3CC320AF9624}">
   <dimension ref="F8:AJ26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12:AC12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2353,18 +2353,18 @@
       <c r="X9" s="19">
         <v>33</v>
       </c>
-      <c r="Z9" s="33" t="s">
+      <c r="Z9" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="34"/>
-      <c r="AC9" s="35"/>
-      <c r="AE9" s="33" t="s">
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="28"/>
+      <c r="AE9" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="AF9" s="34"/>
-      <c r="AG9" s="34"/>
-      <c r="AH9" s="35"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="28"/>
       <c r="AI9" s="24"/>
       <c r="AJ9" s="24"/>
     </row>
@@ -2424,20 +2424,20 @@
       <c r="X10" s="18">
         <v>40</v>
       </c>
-      <c r="Z10" s="26">
+      <c r="Z10" s="29">
         <f>AVERAGE((I10,I16,I22))</f>
         <v>50.657794547354875</v>
       </c>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="28"/>
-      <c r="AE10" s="26">
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="31"/>
+      <c r="AE10" s="29">
         <f>_xlfn.STDEV.P((I10,I16,I22))</f>
         <v>1.6028353405426132</v>
       </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="28"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="31"/>
       <c r="AI10" s="24"/>
       <c r="AJ10" s="24"/>
     </row>
@@ -2497,20 +2497,20 @@
       <c r="X11" s="18">
         <v>89</v>
       </c>
-      <c r="Z11" s="26">
+      <c r="Z11" s="29">
         <f>AVERAGE((I11,I19,I26))</f>
         <v>64.412683967932466</v>
       </c>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="28"/>
-      <c r="AE11" s="26">
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="31"/>
+      <c r="AE11" s="29">
         <f>_xlfn.STDEV.P((I11,I19,I26))</f>
         <v>3.4392912855000688</v>
       </c>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="28"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="31"/>
       <c r="AI11" s="24"/>
       <c r="AJ11" s="24"/>
     </row>
@@ -2570,20 +2570,20 @@
       <c r="X12" s="18">
         <v>110</v>
       </c>
-      <c r="Z12" s="26">
+      <c r="Z12" s="29">
         <f>AVERAGE((I12,I17,I23))</f>
         <v>60.682543056776332</v>
       </c>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="27"/>
-      <c r="AC12" s="28"/>
-      <c r="AE12" s="26">
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="31"/>
+      <c r="AE12" s="29">
         <f>_xlfn.STDEV.P((I12,I17,I23))</f>
         <v>1.6447234117403802</v>
       </c>
-      <c r="AF12" s="27"/>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="28"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="30"/>
+      <c r="AH12" s="31"/>
       <c r="AI12" s="24"/>
       <c r="AJ12" s="24"/>
     </row>
@@ -2605,7 +2605,7 @@
         <f t="shared" ref="J13:J25" si="1">(P13/(P13+S13+V13))*100</f>
         <v>60.353535353535349</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="23">
         <f>T13/(Q13+T13+W13)*100</f>
         <v>67.032967032967022</v>
       </c>
@@ -2643,20 +2643,20 @@
       <c r="X13" s="18">
         <v>175</v>
       </c>
-      <c r="Z13" s="29">
+      <c r="Z13" s="33">
         <f>AVERAGE((I13,I18,I25))</f>
         <v>62.810523228093551</v>
       </c>
-      <c r="AA13" s="30"/>
-      <c r="AB13" s="30"/>
-      <c r="AC13" s="31"/>
-      <c r="AE13" s="29">
+      <c r="AA13" s="34"/>
+      <c r="AB13" s="34"/>
+      <c r="AC13" s="35"/>
+      <c r="AE13" s="33">
         <f>_xlfn.STDEV.P((I13,I18,I25))</f>
         <v>3.2095482362690482</v>
       </c>
-      <c r="AF13" s="30"/>
-      <c r="AG13" s="30"/>
-      <c r="AH13" s="31"/>
+      <c r="AF13" s="34"/>
+      <c r="AG13" s="34"/>
+      <c r="AH13" s="35"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
     </row>
@@ -2671,14 +2671,14 @@
         <v>189</v>
       </c>
       <c r="I14" s="23">
-        <f t="shared" si="0"/>
+        <f>(P14+T14+X14)/(SUM(P14:X14))*100</f>
         <v>65.729166666666671</v>
       </c>
       <c r="J14" s="23">
         <f t="shared" si="1"/>
         <v>65.168539325842701</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="16">
         <f t="shared" ref="K14:K25" si="3">T14/(Q14+T14+W14)*100</f>
         <v>63.586956521739133</v>
       </c>
@@ -2716,20 +2716,20 @@
       <c r="X14" s="18">
         <v>165</v>
       </c>
-      <c r="Z14" s="32">
+      <c r="Z14" s="25">
         <f>AVERAGE((I14,I20,I24))</f>
         <v>65.519721730872689</v>
       </c>
-      <c r="AA14" s="32"/>
-      <c r="AB14" s="32"/>
-      <c r="AC14" s="32"/>
-      <c r="AE14" s="32">
+      <c r="AA14" s="25"/>
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="25"/>
+      <c r="AE14" s="25">
         <f>_xlfn.STDEV.P((I14,I20,I24))</f>
         <v>0.89186948400102095</v>
       </c>
-      <c r="AF14" s="32"/>
-      <c r="AG14" s="32"/>
-      <c r="AH14" s="32"/>
+      <c r="AF14" s="25"/>
+      <c r="AG14" s="25"/>
+      <c r="AH14" s="25"/>
       <c r="AI14" s="24"/>
       <c r="AJ14" s="24"/>
     </row>
@@ -2751,15 +2751,15 @@
       <c r="V15" s="18"/>
       <c r="W15" s="18"/>
       <c r="X15" s="18"/>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
+      <c r="Z15" s="32"/>
+      <c r="AA15" s="32"/>
+      <c r="AB15" s="32"/>
+      <c r="AC15" s="32"/>
       <c r="AD15" s="24"/>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="25"/>
-      <c r="AH15" s="25"/>
+      <c r="AE15" s="32"/>
+      <c r="AF15" s="32"/>
+      <c r="AG15" s="32"/>
+      <c r="AH15" s="32"/>
       <c r="AI15" s="24"/>
       <c r="AJ15" s="24"/>
     </row>
@@ -2777,7 +2777,7 @@
         <f>(P16+T16+X16)/(SUM(P16:X16))*100</f>
         <v>50.469238790406678</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="22">
         <f>(P16/(P16+S16+V16))*100</f>
         <v>90.909090909090907</v>
       </c>
@@ -2887,15 +2887,15 @@
       <c r="X17" s="18">
         <v>161</v>
       </c>
-      <c r="Z17" s="25"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="25"/>
-      <c r="AC17" s="25"/>
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="32"/>
+      <c r="AB17" s="32"/>
+      <c r="AC17" s="32"/>
       <c r="AD17" s="24"/>
-      <c r="AE17" s="25"/>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
-      <c r="AH17" s="25"/>
+      <c r="AE17" s="32"/>
+      <c r="AF17" s="32"/>
+      <c r="AG17" s="32"/>
+      <c r="AH17" s="32"/>
       <c r="AI17" s="24"/>
       <c r="AJ17" s="24"/>
     </row>
@@ -2955,15 +2955,15 @@
       <c r="X18" s="18">
         <v>176</v>
       </c>
-      <c r="Z18" s="25"/>
-      <c r="AA18" s="25"/>
-      <c r="AB18" s="25"/>
-      <c r="AC18" s="25"/>
+      <c r="Z18" s="32"/>
+      <c r="AA18" s="32"/>
+      <c r="AB18" s="32"/>
+      <c r="AC18" s="32"/>
       <c r="AD18" s="24"/>
-      <c r="AE18" s="25"/>
-      <c r="AF18" s="25"/>
-      <c r="AG18" s="25"/>
-      <c r="AH18" s="25"/>
+      <c r="AE18" s="32"/>
+      <c r="AF18" s="32"/>
+      <c r="AG18" s="32"/>
+      <c r="AH18" s="32"/>
       <c r="AI18" s="24"/>
       <c r="AJ18" s="24"/>
     </row>
@@ -2981,7 +2981,7 @@
         <f t="shared" ref="I19" si="4">(P19+T19+X19)/(SUM(P19:X19))*100</f>
         <v>63.503649635036496</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="17">
         <f t="shared" ref="J19" si="5">(P19/(P19+S19+V19))*100</f>
         <v>82.872928176795583</v>
       </c>
@@ -3398,6 +3398,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="Z17:AC17"/>
+    <mergeCell ref="AE17:AH17"/>
+    <mergeCell ref="Z18:AC18"/>
+    <mergeCell ref="AE18:AH18"/>
+    <mergeCell ref="Z15:AC15"/>
+    <mergeCell ref="AE15:AH15"/>
+    <mergeCell ref="Z16:AC16"/>
+    <mergeCell ref="AE16:AH16"/>
     <mergeCell ref="Z9:AC9"/>
     <mergeCell ref="AE9:AH9"/>
     <mergeCell ref="Z14:AC14"/>
@@ -3410,14 +3418,6 @@
     <mergeCell ref="AE12:AH12"/>
     <mergeCell ref="Z11:AC11"/>
     <mergeCell ref="AE11:AH11"/>
-    <mergeCell ref="Z17:AC17"/>
-    <mergeCell ref="AE17:AH17"/>
-    <mergeCell ref="Z18:AC18"/>
-    <mergeCell ref="AE18:AH18"/>
-    <mergeCell ref="Z15:AC15"/>
-    <mergeCell ref="AE15:AH15"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="AE16:AH16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3671,15 +3671,15 @@
       <c r="X11" s="18">
         <v>216</v>
       </c>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="37"/>
+      <c r="AB11" s="37"/>
+      <c r="AC11" s="37"/>
       <c r="AD11" s="24"/>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="38"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="38"/>
+      <c r="AE11" s="37"/>
+      <c r="AF11" s="37"/>
+      <c r="AG11" s="37"/>
+      <c r="AH11" s="37"/>
       <c r="AI11" s="24"/>
       <c r="AJ11" s="24"/>
     </row>
@@ -3739,15 +3739,15 @@
       <c r="X12" s="18">
         <v>223</v>
       </c>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="25"/>
-      <c r="AC12" s="25"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="32"/>
+      <c r="AC12" s="32"/>
       <c r="AD12" s="24"/>
-      <c r="AE12" s="25"/>
-      <c r="AF12" s="25"/>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="25"/>
+      <c r="AE12" s="32"/>
+      <c r="AF12" s="32"/>
+      <c r="AG12" s="32"/>
+      <c r="AH12" s="32"/>
       <c r="AI12" s="24"/>
       <c r="AJ12" s="24"/>
     </row>
@@ -3807,15 +3807,15 @@
       <c r="X13" s="18">
         <v>236</v>
       </c>
-      <c r="Z13" s="25"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="25"/>
-      <c r="AC13" s="25"/>
+      <c r="Z13" s="32"/>
+      <c r="AA13" s="32"/>
+      <c r="AB13" s="32"/>
+      <c r="AC13" s="32"/>
       <c r="AD13" s="24"/>
-      <c r="AE13" s="25"/>
-      <c r="AF13" s="25"/>
-      <c r="AG13" s="25"/>
-      <c r="AH13" s="25"/>
+      <c r="AE13" s="32"/>
+      <c r="AF13" s="32"/>
+      <c r="AG13" s="32"/>
+      <c r="AH13" s="32"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
     </row>
@@ -3875,15 +3875,15 @@
       <c r="X14" s="18">
         <v>240</v>
       </c>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="25"/>
-      <c r="AC14" s="25"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="32"/>
       <c r="AD14" s="24"/>
-      <c r="AE14" s="25"/>
-      <c r="AF14" s="25"/>
-      <c r="AG14" s="25"/>
-      <c r="AH14" s="25"/>
+      <c r="AE14" s="32"/>
+      <c r="AF14" s="32"/>
+      <c r="AG14" s="32"/>
+      <c r="AH14" s="32"/>
       <c r="AI14" s="24"/>
       <c r="AJ14" s="24"/>
     </row>
@@ -3905,15 +3905,15 @@
       <c r="V15" s="18"/>
       <c r="W15" s="18"/>
       <c r="X15" s="18"/>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
+      <c r="Z15" s="32"/>
+      <c r="AA15" s="32"/>
+      <c r="AB15" s="32"/>
+      <c r="AC15" s="32"/>
       <c r="AD15" s="24"/>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="25"/>
-      <c r="AH15" s="25"/>
+      <c r="AE15" s="32"/>
+      <c r="AF15" s="32"/>
+      <c r="AG15" s="32"/>
+      <c r="AH15" s="32"/>
       <c r="AI15" s="24"/>
       <c r="AJ15" s="24"/>
     </row>
@@ -3973,15 +3973,15 @@
       <c r="X16" s="18">
         <v>115</v>
       </c>
-      <c r="Z16" s="37"/>
-      <c r="AA16" s="37"/>
-      <c r="AB16" s="37"/>
-      <c r="AC16" s="37"/>
+      <c r="Z16" s="38"/>
+      <c r="AA16" s="38"/>
+      <c r="AB16" s="38"/>
+      <c r="AC16" s="38"/>
       <c r="AD16" s="24"/>
-      <c r="AE16" s="37"/>
-      <c r="AF16" s="37"/>
-      <c r="AG16" s="37"/>
-      <c r="AH16" s="37"/>
+      <c r="AE16" s="38"/>
+      <c r="AF16" s="38"/>
+      <c r="AG16" s="38"/>
+      <c r="AH16" s="38"/>
       <c r="AI16" s="24"/>
       <c r="AJ16" s="24"/>
     </row>
@@ -4705,15 +4705,15 @@
       <c r="X9" s="19">
         <v>33</v>
       </c>
-      <c r="Z9" s="38"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
-      <c r="AC9" s="38"/>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="37"/>
+      <c r="AC9" s="37"/>
       <c r="AD9" s="24"/>
-      <c r="AE9" s="38"/>
-      <c r="AF9" s="38"/>
-      <c r="AG9" s="38"/>
-      <c r="AH9" s="38"/>
+      <c r="AE9" s="37"/>
+      <c r="AF9" s="37"/>
+      <c r="AG9" s="37"/>
+      <c r="AH9" s="37"/>
       <c r="AI9" s="24"/>
       <c r="AJ9" s="24"/>
     </row>
@@ -4773,15 +4773,15 @@
       <c r="X10" s="18">
         <v>38</v>
       </c>
-      <c r="Z10" s="25"/>
-      <c r="AA10" s="25"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="25"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="32"/>
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="32"/>
       <c r="AD10" s="24"/>
-      <c r="AE10" s="25"/>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
-      <c r="AH10" s="25"/>
+      <c r="AE10" s="32"/>
+      <c r="AF10" s="32"/>
+      <c r="AG10" s="32"/>
+      <c r="AH10" s="32"/>
       <c r="AI10" s="24"/>
       <c r="AJ10" s="24"/>
     </row>
@@ -4841,15 +4841,15 @@
       <c r="X11" s="18">
         <v>46</v>
       </c>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="25"/>
-      <c r="AC11" s="25"/>
+      <c r="Z11" s="32"/>
+      <c r="AA11" s="32"/>
+      <c r="AB11" s="32"/>
+      <c r="AC11" s="32"/>
       <c r="AD11" s="24"/>
-      <c r="AE11" s="25"/>
-      <c r="AF11" s="25"/>
-      <c r="AG11" s="25"/>
-      <c r="AH11" s="25"/>
+      <c r="AE11" s="32"/>
+      <c r="AF11" s="32"/>
+      <c r="AG11" s="32"/>
+      <c r="AH11" s="32"/>
       <c r="AI11" s="24"/>
       <c r="AJ11" s="24"/>
     </row>
@@ -4909,15 +4909,15 @@
       <c r="X12" s="18">
         <v>45</v>
       </c>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="25"/>
-      <c r="AC12" s="25"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="32"/>
+      <c r="AC12" s="32"/>
       <c r="AD12" s="24"/>
-      <c r="AE12" s="25"/>
-      <c r="AF12" s="25"/>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="25"/>
+      <c r="AE12" s="32"/>
+      <c r="AF12" s="32"/>
+      <c r="AG12" s="32"/>
+      <c r="AH12" s="32"/>
       <c r="AI12" s="24"/>
       <c r="AJ12" s="24"/>
     </row>
@@ -4977,15 +4977,15 @@
       <c r="X13" s="18">
         <v>48</v>
       </c>
-      <c r="Z13" s="37"/>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37"/>
-      <c r="AC13" s="37"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="38"/>
+      <c r="AB13" s="38"/>
+      <c r="AC13" s="38"/>
       <c r="AD13" s="24"/>
-      <c r="AE13" s="37"/>
-      <c r="AF13" s="37"/>
-      <c r="AG13" s="37"/>
-      <c r="AH13" s="37"/>
+      <c r="AE13" s="38"/>
+      <c r="AF13" s="38"/>
+      <c r="AG13" s="38"/>
+      <c r="AH13" s="38"/>
       <c r="AI13" s="24"/>
       <c r="AJ13" s="24"/>
     </row>
@@ -5045,15 +5045,15 @@
       <c r="X14" s="18">
         <v>45</v>
       </c>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="25"/>
-      <c r="AC14" s="25"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="32"/>
       <c r="AD14" s="24"/>
-      <c r="AE14" s="25"/>
-      <c r="AF14" s="25"/>
-      <c r="AG14" s="25"/>
-      <c r="AH14" s="25"/>
+      <c r="AE14" s="32"/>
+      <c r="AF14" s="32"/>
+      <c r="AG14" s="32"/>
+      <c r="AH14" s="32"/>
       <c r="AI14" s="24"/>
       <c r="AJ14" s="24"/>
     </row>
@@ -5829,18 +5829,18 @@
       <c r="X9" s="19">
         <v>33</v>
       </c>
-      <c r="Z9" s="33" t="s">
+      <c r="Z9" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="34"/>
-      <c r="AC9" s="35"/>
-      <c r="AE9" s="33" t="s">
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="28"/>
+      <c r="AE9" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="AF9" s="34"/>
-      <c r="AG9" s="34"/>
-      <c r="AH9" s="35"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="28"/>
     </row>
     <row r="10" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F10" s="3" t="s">
@@ -5898,20 +5898,20 @@
       <c r="X10" s="18">
         <v>38</v>
       </c>
-      <c r="Z10" s="26">
+      <c r="Z10" s="29">
         <f>AVERAGE((I10,I20,I32))</f>
         <v>67.835587550901678</v>
       </c>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="28"/>
-      <c r="AE10" s="26">
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="31"/>
+      <c r="AE10" s="29">
         <f>_xlfn.STDEV.P((I10,I20,I32))</f>
         <v>6.0665932688755992</v>
       </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="28"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="31"/>
     </row>
     <row r="11" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F11" s="3" t="s">
@@ -5969,20 +5969,20 @@
       <c r="X11" s="18">
         <v>37</v>
       </c>
-      <c r="Z11" s="26">
+      <c r="Z11" s="29">
         <f>AVERAGE((I11,I21,I33))</f>
         <v>68.704552065154147</v>
       </c>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="28"/>
-      <c r="AE11" s="26">
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="31"/>
+      <c r="AE11" s="29">
         <f>_xlfn.STDEV.P((I11,I21,I33))</f>
         <v>5.9140778565586931</v>
       </c>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="28"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="31"/>
     </row>
     <row r="12" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F12" s="3" t="s">
@@ -6040,20 +6040,20 @@
       <c r="X12" s="18">
         <v>37</v>
       </c>
-      <c r="Z12" s="26">
+      <c r="Z12" s="29">
         <f>AVERAGE((I12,I22,I31))</f>
         <v>68.702734147760324</v>
       </c>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="27"/>
-      <c r="AC12" s="28"/>
-      <c r="AE12" s="26">
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="31"/>
+      <c r="AE12" s="29">
         <f>_xlfn.STDEV.P((I12,I22,I31))</f>
         <v>5.4930297078598143</v>
       </c>
-      <c r="AF12" s="27"/>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="28"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="30"/>
+      <c r="AH12" s="31"/>
     </row>
     <row r="13" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F13" s="3" t="s">
@@ -6111,20 +6111,20 @@
       <c r="X13" s="18">
         <v>40</v>
       </c>
-      <c r="Z13" s="26">
+      <c r="Z13" s="29">
         <f>AVERAGE((I13,I23,I30))</f>
         <v>68.69818935427574</v>
       </c>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="28"/>
-      <c r="AE13" s="26">
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="31"/>
+      <c r="AE13" s="29">
         <f>_xlfn.STDEV.P((I13,I23,I30))</f>
         <v>5.4149035379718242</v>
       </c>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="28"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="31"/>
     </row>
     <row r="14" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F14" s="9" t="s">
@@ -6182,20 +6182,20 @@
       <c r="X14" s="18">
         <v>45</v>
       </c>
-      <c r="Z14" s="26">
+      <c r="Z14" s="29">
         <f>AVERAGE((I25,I14,I35))</f>
         <v>81.920811518324612</v>
       </c>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="27"/>
-      <c r="AC14" s="28"/>
-      <c r="AE14" s="26">
+      <c r="AA14" s="30"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="31"/>
+      <c r="AE14" s="29">
         <f>_xlfn.STDEV.P((I25,I14,I35))</f>
         <v>7.8892039469456838</v>
       </c>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="28"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="31"/>
     </row>
     <row r="15" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="9" t="s">
@@ -6253,20 +6253,20 @@
       <c r="X15" s="18">
         <v>42</v>
       </c>
-      <c r="Z15" s="26">
+      <c r="Z15" s="29">
         <f>AVERAGE((I15,I28,I34))</f>
         <v>81.567226585223963</v>
       </c>
-      <c r="AA15" s="27"/>
-      <c r="AB15" s="27"/>
-      <c r="AC15" s="28"/>
-      <c r="AE15" s="26">
+      <c r="AA15" s="30"/>
+      <c r="AB15" s="30"/>
+      <c r="AC15" s="31"/>
+      <c r="AE15" s="29">
         <f>_xlfn.STDEV.P((I15,I28,I34))</f>
         <v>7.9095836181871686</v>
       </c>
-      <c r="AF15" s="27"/>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="28"/>
+      <c r="AF15" s="30"/>
+      <c r="AG15" s="30"/>
+      <c r="AH15" s="31"/>
     </row>
     <row r="16" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F16" s="11" t="s">
@@ -6324,20 +6324,20 @@
       <c r="X16" s="18">
         <v>47</v>
       </c>
-      <c r="Z16" s="26">
+      <c r="Z16" s="29">
         <f>AVERAGE((I16,I24,I37))</f>
         <v>82.445280686445614</v>
       </c>
-      <c r="AA16" s="27"/>
-      <c r="AB16" s="27"/>
-      <c r="AC16" s="28"/>
-      <c r="AE16" s="26">
+      <c r="AA16" s="30"/>
+      <c r="AB16" s="30"/>
+      <c r="AC16" s="31"/>
+      <c r="AE16" s="29">
         <f>_xlfn.STDEV.P((I16,I24,I37))</f>
         <v>7.1538811074596307</v>
       </c>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="28"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="30"/>
+      <c r="AH16" s="31"/>
     </row>
     <row r="17" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F17" s="11" t="s">
@@ -6395,20 +6395,20 @@
       <c r="X17" s="18">
         <v>49</v>
       </c>
-      <c r="Z17" s="26">
+      <c r="Z17" s="29">
         <f>AVERAGE((I17,I27,I36))</f>
         <v>84.35227603257708</v>
       </c>
-      <c r="AA17" s="27"/>
-      <c r="AB17" s="27"/>
-      <c r="AC17" s="28"/>
-      <c r="AE17" s="26">
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="31"/>
+      <c r="AE17" s="29">
         <f>_xlfn.STDEV.P((I17,I27,I36))</f>
         <v>5.2144280394799756</v>
       </c>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
-      <c r="AH17" s="28"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="31"/>
     </row>
     <row r="18" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F18" s="11" t="s">
@@ -7547,18 +7547,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="AE9:AH9"/>
-    <mergeCell ref="Z10:AC10"/>
-    <mergeCell ref="AE10:AH10"/>
-    <mergeCell ref="Z11:AC11"/>
-    <mergeCell ref="AE11:AH11"/>
-    <mergeCell ref="Z12:AC12"/>
-    <mergeCell ref="AE12:AH12"/>
-    <mergeCell ref="Z13:AC13"/>
-    <mergeCell ref="AE13:AH13"/>
-    <mergeCell ref="Z14:AC14"/>
-    <mergeCell ref="AE14:AH14"/>
     <mergeCell ref="Z18:AC18"/>
     <mergeCell ref="AE18:AH18"/>
     <mergeCell ref="Z15:AC15"/>
@@ -7567,6 +7555,18 @@
     <mergeCell ref="AE16:AH16"/>
     <mergeCell ref="Z17:AC17"/>
     <mergeCell ref="AE17:AH17"/>
+    <mergeCell ref="Z12:AC12"/>
+    <mergeCell ref="AE12:AH12"/>
+    <mergeCell ref="Z13:AC13"/>
+    <mergeCell ref="AE13:AH13"/>
+    <mergeCell ref="Z14:AC14"/>
+    <mergeCell ref="AE14:AH14"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="AE9:AH9"/>
+    <mergeCell ref="Z10:AC10"/>
+    <mergeCell ref="AE10:AH10"/>
+    <mergeCell ref="Z11:AC11"/>
+    <mergeCell ref="AE11:AH11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -7684,18 +7684,18 @@
       <c r="X9" s="19">
         <v>33</v>
       </c>
-      <c r="Z9" s="33" t="s">
+      <c r="Z9" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="34"/>
-      <c r="AC9" s="35"/>
-      <c r="AE9" s="33" t="s">
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="28"/>
+      <c r="AE9" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="AF9" s="34"/>
-      <c r="AG9" s="34"/>
-      <c r="AH9" s="35"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="28"/>
     </row>
     <row r="10" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F10" s="3" t="s">
@@ -7753,20 +7753,20 @@
       <c r="X10" s="18">
         <v>48</v>
       </c>
-      <c r="Z10" s="26">
+      <c r="Z10" s="29">
         <f>AVERAGE((I10,I21,I31))</f>
         <v>39.47046151520059</v>
       </c>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="28"/>
-      <c r="AE10" s="26">
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="31"/>
+      <c r="AE10" s="29">
         <f>_xlfn.STDEV.P((I10,I21,I31))</f>
         <v>5.9358847866159721</v>
       </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="28"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="31"/>
     </row>
     <row r="11" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F11" s="3" t="s">
@@ -7824,20 +7824,20 @@
       <c r="X11" s="18">
         <v>263</v>
       </c>
-      <c r="Z11" s="26">
+      <c r="Z11" s="29">
         <f>AVERAGE((I11,I20,I32))</f>
         <v>41.485191498925396</v>
       </c>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="28"/>
-      <c r="AE11" s="26">
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="31"/>
+      <c r="AE11" s="29">
         <f>_xlfn.STDEV.P((I11,I20,I32))</f>
         <v>6.9075546798479088</v>
       </c>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="28"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="31"/>
     </row>
     <row r="12" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F12" s="3" t="s">
@@ -7895,20 +7895,20 @@
       <c r="X12" s="18">
         <v>167</v>
       </c>
-      <c r="Z12" s="26">
+      <c r="Z12" s="29">
         <f>AVERAGE((I12,I22,I33))</f>
         <v>45.941592683684348</v>
       </c>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="27"/>
-      <c r="AC12" s="28"/>
-      <c r="AE12" s="26">
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="31"/>
+      <c r="AE12" s="29">
         <f>_xlfn.STDEV.P((I12,I22,I33))</f>
         <v>7.9060884593006486</v>
       </c>
-      <c r="AF12" s="27"/>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="28"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="30"/>
+      <c r="AH12" s="31"/>
     </row>
     <row r="13" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F13" s="3" t="s">
@@ -7966,20 +7966,20 @@
       <c r="X13" s="18">
         <v>212</v>
       </c>
-      <c r="Z13" s="26">
+      <c r="Z13" s="29">
         <f>AVERAGE((I13,I23,I30))</f>
         <v>41.087605382339682</v>
       </c>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="28"/>
-      <c r="AE13" s="26">
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="31"/>
+      <c r="AE13" s="29">
         <f>_xlfn.STDEV.P((I13,I23,I30))</f>
         <v>4.0598851254844215</v>
       </c>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="28"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="31"/>
     </row>
     <row r="14" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F14" s="11" t="s">
@@ -8037,20 +8037,20 @@
       <c r="X14" s="18">
         <v>188</v>
       </c>
-      <c r="Z14" s="26">
+      <c r="Z14" s="29">
         <f>AVERAGE((I14,I24,I35))</f>
         <v>65.103159893019253</v>
       </c>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="27"/>
-      <c r="AC14" s="28"/>
-      <c r="AE14" s="26">
+      <c r="AA14" s="30"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="31"/>
+      <c r="AE14" s="29">
         <f>_xlfn.STDEV.P((I14,I24,I35))</f>
         <v>2.1992237349466821</v>
       </c>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="28"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="31"/>
     </row>
     <row r="15" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="9" t="s">
@@ -8108,20 +8108,20 @@
       <c r="X15" s="18">
         <v>209</v>
       </c>
-      <c r="Z15" s="26">
+      <c r="Z15" s="29">
         <f>AVERAGE((I15,I25,I36))</f>
         <v>66.205638640832362</v>
       </c>
-      <c r="AA15" s="27"/>
-      <c r="AB15" s="27"/>
-      <c r="AC15" s="28"/>
-      <c r="AE15" s="26">
+      <c r="AA15" s="30"/>
+      <c r="AB15" s="30"/>
+      <c r="AC15" s="31"/>
+      <c r="AE15" s="29">
         <f>_xlfn.STDEV.P((I15,I25,I36))</f>
         <v>2.3408382952249802</v>
       </c>
-      <c r="AF15" s="27"/>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="28"/>
+      <c r="AF15" s="30"/>
+      <c r="AG15" s="30"/>
+      <c r="AH15" s="31"/>
     </row>
     <row r="16" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F16" s="11" t="s">
@@ -8179,20 +8179,20 @@
       <c r="X16" s="18">
         <v>238</v>
       </c>
-      <c r="Z16" s="26">
+      <c r="Z16" s="29">
         <f>AVERAGE((I16,I28,I38))</f>
         <v>70.152745248619837</v>
       </c>
-      <c r="AA16" s="27"/>
-      <c r="AB16" s="27"/>
-      <c r="AC16" s="28"/>
-      <c r="AE16" s="26">
+      <c r="AA16" s="30"/>
+      <c r="AB16" s="30"/>
+      <c r="AC16" s="31"/>
+      <c r="AE16" s="29">
         <f>_xlfn.STDEV.P((I16,I28,I38))</f>
         <v>3.9656122249328152</v>
       </c>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="28"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="30"/>
+      <c r="AH16" s="31"/>
     </row>
     <row r="17" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="11" t="s">
@@ -8321,20 +8321,20 @@
       <c r="X18" s="18">
         <v>205</v>
       </c>
-      <c r="Z18" s="26">
+      <c r="Z18" s="29">
         <f>AVERAGE((I34,I26,I18))</f>
         <v>66.525459980491618</v>
       </c>
-      <c r="AA18" s="27"/>
-      <c r="AB18" s="27"/>
-      <c r="AC18" s="28"/>
-      <c r="AE18" s="26">
+      <c r="AA18" s="30"/>
+      <c r="AB18" s="30"/>
+      <c r="AC18" s="31"/>
+      <c r="AE18" s="29">
         <f>_xlfn.STDEV.P((I34,I26,I18))</f>
         <v>1.6044891226048548</v>
       </c>
-      <c r="AF18" s="27"/>
-      <c r="AG18" s="27"/>
-      <c r="AH18" s="28"/>
+      <c r="AF18" s="30"/>
+      <c r="AG18" s="30"/>
+      <c r="AH18" s="31"/>
     </row>
     <row r="19" spans="6:34" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F19" s="13"/>
@@ -9402,6 +9402,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="Z16:AC16"/>
+    <mergeCell ref="AE16:AH16"/>
+    <mergeCell ref="Z17:AC17"/>
+    <mergeCell ref="AE17:AH17"/>
+    <mergeCell ref="Z18:AC18"/>
+    <mergeCell ref="AE18:AH18"/>
+    <mergeCell ref="Z13:AC13"/>
+    <mergeCell ref="AE13:AH13"/>
+    <mergeCell ref="Z14:AC14"/>
+    <mergeCell ref="AE14:AH14"/>
+    <mergeCell ref="Z15:AC15"/>
+    <mergeCell ref="AE15:AH15"/>
     <mergeCell ref="Z12:AC12"/>
     <mergeCell ref="AE12:AH12"/>
     <mergeCell ref="Z9:AC9"/>
@@ -9410,18 +9422,6 @@
     <mergeCell ref="AE10:AH10"/>
     <mergeCell ref="Z11:AC11"/>
     <mergeCell ref="AE11:AH11"/>
-    <mergeCell ref="Z13:AC13"/>
-    <mergeCell ref="AE13:AH13"/>
-    <mergeCell ref="Z14:AC14"/>
-    <mergeCell ref="AE14:AH14"/>
-    <mergeCell ref="Z15:AC15"/>
-    <mergeCell ref="AE15:AH15"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="AE16:AH16"/>
-    <mergeCell ref="Z17:AC17"/>
-    <mergeCell ref="AE17:AH17"/>
-    <mergeCell ref="Z18:AC18"/>
-    <mergeCell ref="AE18:AH18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -9470,17 +9470,17 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="5"/>
-      <c r="P8" s="46" t="s">
+      <c r="P8" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
-      <c r="W8" s="46"/>
-      <c r="X8" s="46"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="45"/>
+      <c r="X8" s="45"/>
     </row>
     <row r="9" spans="6:34" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F9" s="7" t="s">
@@ -9534,18 +9534,18 @@
       <c r="X9" s="19">
         <v>33</v>
       </c>
-      <c r="Z9" s="33" t="s">
+      <c r="Z9" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="34"/>
-      <c r="AC9" s="35"/>
-      <c r="AE9" s="33" t="s">
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="28"/>
+      <c r="AE9" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="AF9" s="34"/>
-      <c r="AG9" s="34"/>
-      <c r="AH9" s="35"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="28"/>
     </row>
     <row r="10" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F10" s="3" t="s">
@@ -9603,20 +9603,20 @@
       <c r="X10" s="18">
         <v>404</v>
       </c>
-      <c r="Z10" s="26">
+      <c r="Z10" s="29">
         <f>AVERAGE((I10,I20,I30))</f>
         <v>38.830060529780788</v>
       </c>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="28"/>
-      <c r="AE10" s="26">
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="31"/>
+      <c r="AE10" s="29">
         <f>_xlfn.STDEV.P(I10,I20,I30)</f>
         <v>4.2103894624709355</v>
       </c>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="28"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="31"/>
     </row>
     <row r="11" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F11" s="3" t="s">
@@ -9674,20 +9674,20 @@
       <c r="X11" s="18">
         <v>192</v>
       </c>
-      <c r="Z11" s="26">
+      <c r="Z11" s="29">
         <f>AVERAGE((I11,I21,I32))</f>
         <v>41.359777268732444</v>
       </c>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="28"/>
-      <c r="AE11" s="26">
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="31"/>
+      <c r="AE11" s="29">
         <f>_xlfn.STDEV.P((I11,I21,I32))</f>
         <v>2.2173918482030843</v>
       </c>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="28"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="31"/>
     </row>
     <row r="12" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F12" s="3" t="s">
@@ -9745,20 +9745,20 @@
       <c r="X12" s="18">
         <v>322</v>
       </c>
-      <c r="Z12" s="26">
+      <c r="Z12" s="29">
         <f>AVERAGE((I12,I22,I31))</f>
         <v>40.233722919358677</v>
       </c>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="27"/>
-      <c r="AC12" s="28"/>
-      <c r="AE12" s="26">
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="31"/>
+      <c r="AE12" s="29">
         <f>_xlfn.STDEV.P((I12,I22,I31))</f>
         <v>3.1460873986200091</v>
       </c>
-      <c r="AF12" s="27"/>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="28"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="30"/>
+      <c r="AH12" s="31"/>
     </row>
     <row r="13" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F13" s="3" t="s">
@@ -9816,20 +9816,20 @@
       <c r="X13" s="18">
         <v>463</v>
       </c>
-      <c r="Z13" s="26">
+      <c r="Z13" s="29">
         <f>AVERAGE((I13,I23,I33))</f>
         <v>42.63360936666836</v>
       </c>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="28"/>
-      <c r="AE13" s="26">
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="31"/>
+      <c r="AE13" s="29">
         <f>_xlfn.STDEV.P((I13,I23,I33))</f>
         <v>3.3524165736582754</v>
       </c>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="28"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="31"/>
     </row>
     <row r="14" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F14" s="11" t="s">
@@ -9887,20 +9887,20 @@
       <c r="X14" s="18">
         <v>159</v>
       </c>
-      <c r="Z14" s="26">
+      <c r="Z14" s="29">
         <f>AVERAGE((I14,I26,I34))</f>
         <v>57.647199557967419</v>
       </c>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="27"/>
-      <c r="AC14" s="28"/>
-      <c r="AE14" s="26">
+      <c r="AA14" s="30"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="31"/>
+      <c r="AE14" s="29">
         <f>_xlfn.STDEV.P((I14,I26,I34))</f>
         <v>3.5382779095587118</v>
       </c>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="28"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="31"/>
     </row>
     <row r="15" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="11" t="s">
@@ -9958,20 +9958,20 @@
       <c r="X15" s="18">
         <v>250</v>
       </c>
-      <c r="Z15" s="26">
+      <c r="Z15" s="29">
         <f>AVERAGE((I15,I27,I38))</f>
         <v>63.748601018731335</v>
       </c>
-      <c r="AA15" s="27"/>
-      <c r="AB15" s="27"/>
-      <c r="AC15" s="28"/>
-      <c r="AE15" s="26">
+      <c r="AA15" s="30"/>
+      <c r="AB15" s="30"/>
+      <c r="AC15" s="31"/>
+      <c r="AE15" s="29">
         <f>_xlfn.STDEV.P((I15,I27,I38))</f>
         <v>2.1741814421862391</v>
       </c>
-      <c r="AF15" s="27"/>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="28"/>
+      <c r="AF15" s="30"/>
+      <c r="AG15" s="30"/>
+      <c r="AH15" s="31"/>
     </row>
     <row r="16" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F16" s="9" t="s">
@@ -10100,20 +10100,20 @@
       <c r="X17" s="18">
         <v>191</v>
       </c>
-      <c r="Z17" s="26">
+      <c r="Z17" s="29">
         <f>AVERAGE((I17,I25,I35))</f>
         <v>62.979479409118845</v>
       </c>
-      <c r="AA17" s="27"/>
-      <c r="AB17" s="27"/>
-      <c r="AC17" s="28"/>
-      <c r="AE17" s="26">
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="31"/>
+      <c r="AE17" s="29">
         <f>_xlfn.STDEV.P((I17,I25,I35))</f>
         <v>2.1504491992080523</v>
       </c>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
-      <c r="AH17" s="28"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="31"/>
     </row>
     <row r="18" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F18" s="9" t="s">
@@ -10171,20 +10171,20 @@
       <c r="X18" s="18">
         <v>193</v>
       </c>
-      <c r="Z18" s="26">
+      <c r="Z18" s="29">
         <f>AVERAGE((I18,I24,I36))</f>
         <v>63.849498467110834</v>
       </c>
-      <c r="AA18" s="27"/>
-      <c r="AB18" s="27"/>
-      <c r="AC18" s="28"/>
-      <c r="AE18" s="26">
+      <c r="AA18" s="30"/>
+      <c r="AB18" s="30"/>
+      <c r="AC18" s="31"/>
+      <c r="AE18" s="29">
         <f>_xlfn.STDEV.P((I18,I24,I36))</f>
         <v>2.85539171234905</v>
       </c>
-      <c r="AF18" s="27"/>
-      <c r="AG18" s="27"/>
-      <c r="AH18" s="28"/>
+      <c r="AF18" s="30"/>
+      <c r="AG18" s="30"/>
+      <c r="AH18" s="31"/>
     </row>
     <row r="19" spans="6:34" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F19" s="13"/>
@@ -10204,10 +10204,10 @@
       <c r="V19" s="18"/>
       <c r="W19" s="18"/>
       <c r="X19" s="18"/>
-      <c r="Z19" s="45"/>
-      <c r="AA19" s="45"/>
-      <c r="AB19" s="45"/>
-      <c r="AC19" s="45"/>
+      <c r="Z19" s="46"/>
+      <c r="AA19" s="46"/>
+      <c r="AB19" s="46"/>
+      <c r="AC19" s="46"/>
     </row>
     <row r="20" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F20" s="3" t="s">
@@ -10265,10 +10265,10 @@
       <c r="X20" s="18">
         <v>392</v>
       </c>
-      <c r="Z20" s="45"/>
-      <c r="AA20" s="45"/>
-      <c r="AB20" s="45"/>
-      <c r="AC20" s="45"/>
+      <c r="Z20" s="46"/>
+      <c r="AA20" s="46"/>
+      <c r="AB20" s="46"/>
+      <c r="AC20" s="46"/>
     </row>
     <row r="21" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F21" s="3" t="s">
@@ -10326,10 +10326,10 @@
       <c r="X21" s="18">
         <v>539</v>
       </c>
-      <c r="Z21" s="45"/>
-      <c r="AA21" s="45"/>
-      <c r="AB21" s="45"/>
-      <c r="AC21" s="45"/>
+      <c r="Z21" s="46"/>
+      <c r="AA21" s="46"/>
+      <c r="AB21" s="46"/>
+      <c r="AC21" s="46"/>
     </row>
     <row r="22" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F22" s="3" t="s">
@@ -10387,10 +10387,10 @@
       <c r="X22" s="18">
         <v>329</v>
       </c>
-      <c r="Z22" s="45"/>
-      <c r="AA22" s="45"/>
-      <c r="AB22" s="45"/>
-      <c r="AC22" s="45"/>
+      <c r="Z22" s="46"/>
+      <c r="AA22" s="46"/>
+      <c r="AB22" s="46"/>
+      <c r="AC22" s="46"/>
     </row>
     <row r="23" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F23" s="3" t="s">
@@ -10448,10 +10448,10 @@
       <c r="X23" s="18">
         <v>416</v>
       </c>
-      <c r="Z23" s="45"/>
-      <c r="AA23" s="45"/>
-      <c r="AB23" s="45"/>
-      <c r="AC23" s="45"/>
+      <c r="Z23" s="46"/>
+      <c r="AA23" s="46"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="46"/>
     </row>
     <row r="24" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F24" s="9" t="s">
@@ -10509,10 +10509,10 @@
       <c r="X24" s="18">
         <v>216</v>
       </c>
-      <c r="Z24" s="45"/>
-      <c r="AA24" s="45"/>
-      <c r="AB24" s="45"/>
-      <c r="AC24" s="45"/>
+      <c r="Z24" s="46"/>
+      <c r="AA24" s="46"/>
+      <c r="AB24" s="46"/>
+      <c r="AC24" s="46"/>
     </row>
     <row r="25" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F25" s="11" t="s">
@@ -10570,10 +10570,10 @@
       <c r="X25" s="18">
         <v>150</v>
       </c>
-      <c r="Z25" s="45"/>
-      <c r="AA25" s="45"/>
-      <c r="AB25" s="45"/>
-      <c r="AC25" s="45"/>
+      <c r="Z25" s="46"/>
+      <c r="AA25" s="46"/>
+      <c r="AB25" s="46"/>
+      <c r="AC25" s="46"/>
     </row>
     <row r="26" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F26" s="11" t="s">
@@ -10631,10 +10631,10 @@
       <c r="X26" s="18">
         <v>172</v>
       </c>
-      <c r="Z26" s="45"/>
-      <c r="AA26" s="45"/>
-      <c r="AB26" s="45"/>
-      <c r="AC26" s="45"/>
+      <c r="Z26" s="46"/>
+      <c r="AA26" s="46"/>
+      <c r="AB26" s="46"/>
+      <c r="AC26" s="46"/>
     </row>
     <row r="27" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F27" s="11" t="s">
@@ -10692,10 +10692,10 @@
       <c r="X27" s="18">
         <v>183</v>
       </c>
-      <c r="Z27" s="45"/>
-      <c r="AA27" s="45"/>
-      <c r="AB27" s="45"/>
-      <c r="AC27" s="45"/>
+      <c r="Z27" s="46"/>
+      <c r="AA27" s="46"/>
+      <c r="AB27" s="46"/>
+      <c r="AC27" s="46"/>
     </row>
     <row r="28" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F28" s="9" t="s">
@@ -10753,10 +10753,10 @@
       <c r="X28" s="18">
         <v>193</v>
       </c>
-      <c r="Z28" s="45"/>
-      <c r="AA28" s="45"/>
-      <c r="AB28" s="45"/>
-      <c r="AC28" s="45"/>
+      <c r="Z28" s="46"/>
+      <c r="AA28" s="46"/>
+      <c r="AB28" s="46"/>
+      <c r="AC28" s="46"/>
     </row>
     <row r="29" spans="6:34" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F29" s="13"/>
@@ -10776,10 +10776,10 @@
       <c r="V29" s="18"/>
       <c r="W29" s="18"/>
       <c r="X29" s="18"/>
-      <c r="Z29" s="45"/>
-      <c r="AA29" s="45"/>
-      <c r="AB29" s="45"/>
-      <c r="AC29" s="45"/>
+      <c r="Z29" s="46"/>
+      <c r="AA29" s="46"/>
+      <c r="AB29" s="46"/>
+      <c r="AC29" s="46"/>
     </row>
     <row r="30" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F30" s="3" t="s">
@@ -10837,10 +10837,10 @@
       <c r="X30" s="18">
         <v>1</v>
       </c>
-      <c r="Z30" s="45"/>
-      <c r="AA30" s="45"/>
-      <c r="AB30" s="45"/>
-      <c r="AC30" s="45"/>
+      <c r="Z30" s="46"/>
+      <c r="AA30" s="46"/>
+      <c r="AB30" s="46"/>
+      <c r="AC30" s="46"/>
     </row>
     <row r="31" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F31" s="3" t="s">
@@ -10898,10 +10898,10 @@
       <c r="X31" s="18">
         <v>16</v>
       </c>
-      <c r="Z31" s="45"/>
-      <c r="AA31" s="45"/>
-      <c r="AB31" s="45"/>
-      <c r="AC31" s="45"/>
+      <c r="Z31" s="46"/>
+      <c r="AA31" s="46"/>
+      <c r="AB31" s="46"/>
+      <c r="AC31" s="46"/>
     </row>
     <row r="32" spans="6:34" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F32" s="3" t="s">
@@ -10959,10 +10959,10 @@
       <c r="X32" s="18">
         <v>30</v>
       </c>
-      <c r="Z32" s="45"/>
-      <c r="AA32" s="45"/>
-      <c r="AB32" s="45"/>
-      <c r="AC32" s="45"/>
+      <c r="Z32" s="46"/>
+      <c r="AA32" s="46"/>
+      <c r="AB32" s="46"/>
+      <c r="AC32" s="46"/>
     </row>
     <row r="33" spans="6:29" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F33" s="3" t="s">
@@ -11020,10 +11020,10 @@
       <c r="X33" s="18">
         <v>14</v>
       </c>
-      <c r="Z33" s="45"/>
-      <c r="AA33" s="45"/>
-      <c r="AB33" s="45"/>
-      <c r="AC33" s="45"/>
+      <c r="Z33" s="46"/>
+      <c r="AA33" s="46"/>
+      <c r="AB33" s="46"/>
+      <c r="AC33" s="46"/>
     </row>
     <row r="34" spans="6:29" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F34" s="11" t="s">
@@ -11081,10 +11081,10 @@
       <c r="X34" s="18">
         <v>59</v>
       </c>
-      <c r="Z34" s="45"/>
-      <c r="AA34" s="45"/>
-      <c r="AB34" s="45"/>
-      <c r="AC34" s="45"/>
+      <c r="Z34" s="46"/>
+      <c r="AA34" s="46"/>
+      <c r="AB34" s="46"/>
+      <c r="AC34" s="46"/>
     </row>
     <row r="35" spans="6:29" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F35" s="11" t="s">
@@ -11142,10 +11142,10 @@
       <c r="X35" s="18">
         <v>211</v>
       </c>
-      <c r="Z35" s="45"/>
-      <c r="AA35" s="45"/>
-      <c r="AB35" s="45"/>
-      <c r="AC35" s="45"/>
+      <c r="Z35" s="46"/>
+      <c r="AA35" s="46"/>
+      <c r="AB35" s="46"/>
+      <c r="AC35" s="46"/>
     </row>
     <row r="36" spans="6:29" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F36" s="9" t="s">
@@ -11203,10 +11203,10 @@
       <c r="X36" s="18">
         <v>217</v>
       </c>
-      <c r="Z36" s="45"/>
-      <c r="AA36" s="45"/>
-      <c r="AB36" s="45"/>
-      <c r="AC36" s="45"/>
+      <c r="Z36" s="46"/>
+      <c r="AA36" s="46"/>
+      <c r="AB36" s="46"/>
+      <c r="AC36" s="46"/>
     </row>
     <row r="37" spans="6:29" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F37" s="9" t="s">
@@ -11264,10 +11264,10 @@
       <c r="X37" s="18">
         <v>248</v>
       </c>
-      <c r="Z37" s="45"/>
-      <c r="AA37" s="45"/>
-      <c r="AB37" s="45"/>
-      <c r="AC37" s="45"/>
+      <c r="Z37" s="46"/>
+      <c r="AA37" s="46"/>
+      <c r="AB37" s="46"/>
+      <c r="AC37" s="46"/>
     </row>
     <row r="38" spans="6:29" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F38" s="11" t="s">
@@ -11325,38 +11325,13 @@
       <c r="X38" s="18">
         <v>203</v>
       </c>
-      <c r="Z38" s="45"/>
-      <c r="AA38" s="45"/>
-      <c r="AB38" s="45"/>
-      <c r="AC38" s="45"/>
+      <c r="Z38" s="46"/>
+      <c r="AA38" s="46"/>
+      <c r="AB38" s="46"/>
+      <c r="AC38" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="P8:X8"/>
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="Z10:AC10"/>
-    <mergeCell ref="Z11:AC11"/>
-    <mergeCell ref="Z12:AC12"/>
-    <mergeCell ref="Z24:AC24"/>
-    <mergeCell ref="Z13:AC13"/>
-    <mergeCell ref="Z14:AC14"/>
-    <mergeCell ref="Z15:AC15"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="Z17:AC17"/>
-    <mergeCell ref="Z18:AC18"/>
-    <mergeCell ref="Z19:AC19"/>
-    <mergeCell ref="Z20:AC20"/>
-    <mergeCell ref="Z21:AC21"/>
-    <mergeCell ref="Z22:AC22"/>
-    <mergeCell ref="Z23:AC23"/>
-    <mergeCell ref="Z35:AC35"/>
-    <mergeCell ref="Z36:AC36"/>
-    <mergeCell ref="Z25:AC25"/>
-    <mergeCell ref="Z26:AC26"/>
-    <mergeCell ref="Z27:AC27"/>
-    <mergeCell ref="Z28:AC28"/>
-    <mergeCell ref="Z29:AC29"/>
-    <mergeCell ref="Z30:AC30"/>
     <mergeCell ref="AE17:AH17"/>
     <mergeCell ref="AE18:AH18"/>
     <mergeCell ref="Z37:AC37"/>
@@ -11373,6 +11348,31 @@
     <mergeCell ref="Z32:AC32"/>
     <mergeCell ref="Z33:AC33"/>
     <mergeCell ref="Z34:AC34"/>
+    <mergeCell ref="Z35:AC35"/>
+    <mergeCell ref="Z36:AC36"/>
+    <mergeCell ref="Z25:AC25"/>
+    <mergeCell ref="Z26:AC26"/>
+    <mergeCell ref="Z27:AC27"/>
+    <mergeCell ref="Z28:AC28"/>
+    <mergeCell ref="Z29:AC29"/>
+    <mergeCell ref="Z30:AC30"/>
+    <mergeCell ref="Z24:AC24"/>
+    <mergeCell ref="Z13:AC13"/>
+    <mergeCell ref="Z14:AC14"/>
+    <mergeCell ref="Z15:AC15"/>
+    <mergeCell ref="Z16:AC16"/>
+    <mergeCell ref="Z17:AC17"/>
+    <mergeCell ref="Z18:AC18"/>
+    <mergeCell ref="Z19:AC19"/>
+    <mergeCell ref="Z20:AC20"/>
+    <mergeCell ref="Z21:AC21"/>
+    <mergeCell ref="Z22:AC22"/>
+    <mergeCell ref="Z23:AC23"/>
+    <mergeCell ref="P8:X8"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="Z10:AC10"/>
+    <mergeCell ref="Z11:AC11"/>
+    <mergeCell ref="Z12:AC12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>